<commit_message>
catch share figure updates
</commit_message>
<xml_diff>
--- a/data/database/processed/catch_share_allocation_database_forloading.xlsx
+++ b/data/database/processed/catch_share_allocation_database_forloading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitchel/Dropbox/Repositories/cc_allocation/data/database/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076D9D6F-EBEA-FE46-A9C9-78790F98938B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E590721B-DEB2-1A4D-81A1-2370ABDD0914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43460" yWindow="-2780" windowWidth="27640" windowHeight="16940" xr2:uid="{F665CF98-F318-1146-88DB-A3A8C8F5368C}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{F665CF98-F318-1146-88DB-A3A8C8F5368C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="78">
   <si>
     <t>share_program</t>
   </si>
@@ -245,13 +245,37 @@
   </si>
   <si>
     <t>recent</t>
+  </si>
+  <si>
+    <t>short_program_name</t>
+  </si>
+  <si>
+    <t>AI Pollock</t>
+  </si>
+  <si>
+    <t>BS AFA Pollock Cooperative (Inshore)</t>
+  </si>
+  <si>
+    <t>BSAI Groundfish Cooperatives (Amendment 80)</t>
+  </si>
+  <si>
+    <t>BSAI King and Tanner Crab</t>
+  </si>
+  <si>
+    <t>Central GOA Rockfish</t>
+  </si>
+  <si>
+    <t>IFQ Halibut and Sablefish</t>
+  </si>
+  <si>
+    <t>West Coast Groundfish Trawl (shoreside sector)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,6 +301,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -314,11 +346,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,77 +666,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8924D8-153C-DF42-A58F-4E2459EE41BB}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="71.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>2005</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
@@ -722,898 +761,964 @@
       <c r="M2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2">
         <v>2010</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>2000</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>2004</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
+      <c r="L3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3">
         <v>2.5</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2">
         <v>2010</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>2000</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>2004</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="2">
-        <v>5</v>
+      <c r="L4" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2">
         <v>1999</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>1995</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>1997</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="2">
-        <v>30</v>
+      <c r="L5" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M5" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2">
         <v>1999</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>1995</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>1997</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="2">
-        <v>17.5</v>
+      <c r="L6" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M6" s="2">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="2">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2">
         <v>2008</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>1998</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>2004</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="2">
-        <v>30</v>
+      <c r="L7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M7" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="F8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2">
         <v>2008</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>1998</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>2004</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="2">
-        <v>20</v>
+      <c r="L8" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M8" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="F9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="2">
         <v>2005</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>1991</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>2000</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="2">
+      <c r="L9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="2">
         <v>1</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="2">
         <v>2005</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>1991</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>2000</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="2">
+      <c r="L10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="2">
         <v>2</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="F11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="2">
         <v>2005</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>1991</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>2000</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="2">
-        <v>60</v>
+      <c r="L11" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M11" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="F12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="2">
         <v>2005</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>1991</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>2000</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" s="2">
-        <v>2</v>
+      <c r="L12" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M12" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="F13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="2">
         <v>2007</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>2000</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>2006</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" s="2">
+      <c r="L13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="2">
         <v>4</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="F14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="2">
         <v>2007</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>2000</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>2006</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="2">
-        <v>30</v>
+      <c r="L14" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M14" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="F15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="2">
         <v>2007</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>2000</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>2006</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" s="2">
-        <v>8</v>
+      <c r="L15" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M15" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="F16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="2">
         <v>2007</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>2000</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>2006</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" s="2">
-        <v>30</v>
+      <c r="L16" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M16" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="2">
         <v>2009</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>2001</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>2005</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" s="2">
-        <v>49</v>
+      <c r="L17" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M17" s="2">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="2">
         <v>2010</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>1999</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>2004</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L18" s="2">
+      <c r="L18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="M18" s="2">
+      <c r="N18" s="2">
         <v>14.7</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="F19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="2">
         <v>2010</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>1999</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>2004</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="2">
+      <c r="L19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="M19" s="2">
+      <c r="N19" s="2">
         <v>14.7</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="F20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="2">
         <v>2015</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>2006</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>2012</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L20" s="2">
-        <v>25</v>
+      <c r="L20" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M20" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="F21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="2">
         <v>2015</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>2006</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>2012</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L21" s="2">
-        <v>25</v>
+      <c r="L21" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M21" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="F22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="2">
         <v>1995</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>1984</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <v>1990</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L22" s="2">
-        <v>1</v>
+      <c r="L22" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="F23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="2">
         <v>1995</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>1984</v>
       </c>
-      <c r="H23" s="2">
+      <c r="I23" s="2">
         <v>1990</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L23" s="2">
-        <v>1</v>
+      <c r="L23" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="2">
+      <c r="F24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="2">
         <v>2010</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>1996</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>2006</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J24" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>18</v>
@@ -1624,446 +1729,479 @@
       <c r="M24" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="F25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="2">
         <v>2024</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>2009</v>
       </c>
-      <c r="H25" s="2">
+      <c r="I25" s="2">
         <v>2019</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L25" s="2">
-        <v>5</v>
+      <c r="L25" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M25" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="2">
+      <c r="F26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="2">
         <v>2024</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>2009</v>
       </c>
-      <c r="H26" s="2">
+      <c r="I26" s="2">
         <v>2019</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K26" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L26" s="2">
-        <v>5</v>
+      <c r="L26" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M26" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="2">
+      <c r="F27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="2">
         <v>2024</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>2009</v>
       </c>
-      <c r="H27" s="2">
+      <c r="I27" s="2">
         <v>2019</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L27" s="2">
-        <v>20</v>
+      <c r="L27" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M27" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="F28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="2">
         <v>2024</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>2009</v>
       </c>
-      <c r="H28" s="2">
+      <c r="I28" s="2">
         <v>2019</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L28" s="2">
-        <v>20</v>
+      <c r="L28" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M28" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="2">
+      <c r="F29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="2">
         <v>2007</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>1990</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>2005</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K29" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L29" s="2">
-        <v>6</v>
+      <c r="L29" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M29" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="2">
+      <c r="F30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="2">
         <v>1990</v>
       </c>
-      <c r="G30" s="2">
+      <c r="H30" s="2">
         <v>1979</v>
       </c>
-      <c r="H30" s="2">
+      <c r="I30" s="2">
         <v>1988</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K30" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L30" s="2">
+      <c r="L30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M30" s="2">
         <v>35</v>
       </c>
-      <c r="M30" s="2">
+      <c r="N30" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="2">
+      <c r="F31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="2">
         <v>1990</v>
       </c>
-      <c r="G31" s="2">
+      <c r="H31" s="2">
         <v>1979</v>
       </c>
-      <c r="H31" s="2">
+      <c r="I31" s="2">
         <v>1988</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L31" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="M31" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="2">
+      <c r="F32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="2">
         <v>2002</v>
       </c>
-      <c r="G32" s="2">
+      <c r="H32" s="2">
         <v>1984</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>1994</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="L32" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="M32" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="2">
+      <c r="G33" s="2">
         <v>2000</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="H33" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="J33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K33" s="2"/>
       <c r="L33" s="2" t="s">
         <v>18</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="2">
+      <c r="F34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="2">
         <v>2011</v>
       </c>
-      <c r="G34" s="2">
+      <c r="H34" s="2">
         <v>1994</v>
       </c>
-      <c r="H34" s="2">
+      <c r="I34" s="2">
         <v>2003</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L34" s="2">
+      <c r="L34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M34" s="2">
         <v>2.5</v>
       </c>
-      <c r="M34" s="2">
+      <c r="N34" s="2">
         <v>17.7</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="2">
+      <c r="F35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="2">
         <v>2011</v>
       </c>
-      <c r="G35" s="2">
+      <c r="H35" s="2">
         <v>1998</v>
       </c>
-      <c r="H35" s="2">
+      <c r="I35" s="2">
         <v>2004</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="J35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="K35" s="2" t="s">
         <v>18</v>
       </c>
@@ -2073,71 +2211,77 @@
       <c r="M35" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="2">
+      <c r="F36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="2">
         <v>2011</v>
       </c>
-      <c r="G36" s="2">
+      <c r="H36" s="2">
         <v>1994</v>
       </c>
-      <c r="H36" s="2">
+      <c r="I36" s="2">
         <v>2003</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K36" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L36" s="2">
+      <c r="L36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M36" s="2">
         <v>3.9</v>
       </c>
-      <c r="M36" s="2">
+      <c r="N36" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F37" s="3">
+      <c r="G37" s="3">
         <v>1992</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I37" s="2" t="s">
@@ -2155,79 +2299,85 @@
       <c r="M37" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="2">
+      <c r="F38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="2">
         <v>1991</v>
       </c>
-      <c r="G38" s="2">
+      <c r="H38" s="2">
         <v>1987</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>1990</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K38" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L38" s="2">
-        <v>49</v>
+      <c r="L38" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="M38" s="2">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="2">
+      <c r="F39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="2">
         <v>1991</v>
       </c>
-      <c r="G39" s="2">
+      <c r="H39" s="2">
         <v>2006</v>
       </c>
-      <c r="H39" s="2">
+      <c r="I39" s="2">
         <v>2011</v>
       </c>
-      <c r="I39" s="3" t="s">
+      <c r="J39" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J39" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="K39" s="2" t="s">
         <v>18</v>
       </c>
@@ -2235,6 +2385,9 @@
         <v>18</v>
       </c>
       <c r="M39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N39" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
somewhat finalized catchshare figures and input tables
</commit_message>
<xml_diff>
--- a/data/database/processed/catch_share_allocation_database_forloading.xlsx
+++ b/data/database/processed/catch_share_allocation_database_forloading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitchel/Dropbox/Repositories/cc_allocation/data/database/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E590721B-DEB2-1A4D-81A1-2370ABDD0914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CE7B6F-03AB-734B-9E7B-72DF45E54577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{F665CF98-F318-1146-88DB-A3A8C8F5368C}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>single</t>
   </si>
   <si>
-    <t>managed by Aleut Corporation</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>Scallop Fishery off Alaska</t>
   </si>
   <si>
-    <t>annual negotiations</t>
-  </si>
-  <si>
     <t>West Coast Groundfish Trawl Catch Share Program (shoreside sector)</t>
   </si>
   <si>
@@ -232,9 +226,6 @@
     <t>Western Alaska Community Development Quota</t>
   </si>
   <si>
-    <t>decennial applications by CDQ groups</t>
-  </si>
-  <si>
     <t>Wreckfish</t>
   </si>
   <si>
@@ -269,6 +260,15 @@
   </si>
   <si>
     <t>West Coast Groundfish Trawl (shoreside sector)</t>
+  </si>
+  <si>
+    <t>Annual negotiations</t>
+  </si>
+  <si>
+    <t>Decennial applications by CDQ groups</t>
+  </si>
+  <si>
+    <t>Managed by Aleut Corporation</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,7 +679,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -738,51 +738,51 @@
         <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="G2" s="2">
         <v>2005</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2">
         <v>2010</v>
@@ -794,13 +794,13 @@
         <v>2004</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M3">
         <v>2.5</v>
@@ -811,22 +811,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2">
         <v>2010</v>
@@ -838,13 +838,13 @@
         <v>2004</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M4" s="2">
         <v>5</v>
@@ -855,10 +855,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -870,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2">
         <v>1999</v>
@@ -882,13 +882,13 @@
         <v>1997</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M5" s="2">
         <v>30</v>
@@ -899,10 +899,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -914,7 +914,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="2">
         <v>1999</v>
@@ -926,13 +926,13 @@
         <v>1997</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M6" s="2">
         <v>17.5</v>
@@ -943,10 +943,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
@@ -955,10 +955,10 @@
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="2">
         <v>2008</v>
@@ -970,13 +970,13 @@
         <v>2004</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M7" s="2">
         <v>30</v>
@@ -987,10 +987,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
@@ -999,10 +999,10 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2">
         <v>2008</v>
@@ -1014,13 +1014,13 @@
         <v>2004</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M8" s="2">
         <v>20</v>
@@ -1031,22 +1031,22 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="2">
         <v>2005</v>
@@ -1058,13 +1058,13 @@
         <v>2000</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M9" s="2">
         <v>1</v>
@@ -1075,22 +1075,22 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="2">
         <v>2005</v>
@@ -1102,13 +1102,13 @@
         <v>2000</v>
       </c>
       <c r="J10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M10" s="2">
         <v>2</v>
@@ -1119,22 +1119,22 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="2">
         <v>2005</v>
@@ -1146,13 +1146,13 @@
         <v>2000</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M11" s="2">
         <v>60</v>
@@ -1163,22 +1163,22 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" s="2">
         <v>2005</v>
@@ -1190,13 +1190,13 @@
         <v>2000</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M12" s="2">
         <v>2</v>
@@ -1207,22 +1207,22 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13" s="2">
         <v>2007</v>
@@ -1234,13 +1234,13 @@
         <v>2006</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M13" s="2">
         <v>4</v>
@@ -1251,22 +1251,22 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="2">
         <v>2007</v>
@@ -1278,13 +1278,13 @@
         <v>2006</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M14" s="2">
         <v>30</v>
@@ -1295,22 +1295,22 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" s="2">
         <v>2007</v>
@@ -1322,13 +1322,13 @@
         <v>2006</v>
       </c>
       <c r="J15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M15" s="2">
         <v>8</v>
@@ -1339,22 +1339,22 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" s="2">
         <v>2007</v>
@@ -1366,13 +1366,13 @@
         <v>2006</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M16" s="2">
         <v>30</v>
@@ -1383,22 +1383,22 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G17" s="2">
         <v>2009</v>
@@ -1410,13 +1410,13 @@
         <v>2005</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M17" s="2">
         <v>49</v>
@@ -1427,22 +1427,22 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" s="2">
         <v>2010</v>
@@ -1454,13 +1454,13 @@
         <v>2004</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M18" s="2">
         <v>2.2999999999999998</v>
@@ -1471,22 +1471,22 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G19" s="2">
         <v>2010</v>
@@ -1498,13 +1498,13 @@
         <v>2004</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M19" s="2">
         <v>2.2999999999999998</v>
@@ -1515,22 +1515,22 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20" s="2">
         <v>2015</v>
@@ -1542,13 +1542,13 @@
         <v>2012</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M20" s="2">
         <v>25</v>
@@ -1559,22 +1559,22 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21" s="2">
         <v>2015</v>
@@ -1586,13 +1586,13 @@
         <v>2012</v>
       </c>
       <c r="J21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M21" s="2">
         <v>25</v>
@@ -1603,22 +1603,22 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G22" s="2">
         <v>1995</v>
@@ -1630,13 +1630,13 @@
         <v>1990</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M22" s="2">
         <v>1</v>
@@ -1647,22 +1647,22 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G23" s="2">
         <v>1995</v>
@@ -1674,13 +1674,13 @@
         <v>1990</v>
       </c>
       <c r="J23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K23" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M23" s="2">
         <v>1</v>
@@ -1691,22 +1691,22 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G24" s="2">
         <v>2010</v>
@@ -1718,27 +1718,27 @@
         <v>2006</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>14</v>
@@ -1750,7 +1750,7 @@
         <v>16</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G25" s="2">
         <v>2024</v>
@@ -1762,13 +1762,13 @@
         <v>2019</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M25" s="2">
         <v>5</v>
@@ -1779,10 +1779,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>14</v>
@@ -1794,7 +1794,7 @@
         <v>16</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G26" s="2">
         <v>2024</v>
@@ -1806,13 +1806,13 @@
         <v>2019</v>
       </c>
       <c r="J26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K26" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L26" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M26" s="2">
         <v>5</v>
@@ -1823,10 +1823,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>14</v>
@@ -1838,7 +1838,7 @@
         <v>16</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G27" s="2">
         <v>2024</v>
@@ -1850,13 +1850,13 @@
         <v>2019</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M27" s="2">
         <v>20</v>
@@ -1867,10 +1867,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>14</v>
@@ -1882,7 +1882,7 @@
         <v>16</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G28" s="2">
         <v>2024</v>
@@ -1894,13 +1894,13 @@
         <v>2019</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M28" s="2">
         <v>20</v>
@@ -1911,22 +1911,22 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G29" s="2">
         <v>2007</v>
@@ -1938,13 +1938,13 @@
         <v>2005</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M29" s="2">
         <v>6</v>
@@ -1955,22 +1955,22 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G30" s="2">
         <v>1990</v>
@@ -1982,13 +1982,13 @@
         <v>1988</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M30" s="2">
         <v>35</v>
@@ -1999,22 +1999,22 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G31" s="2">
         <v>1990</v>
@@ -2026,39 +2026,39 @@
         <v>1988</v>
       </c>
       <c r="J31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K31" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G32" s="2">
         <v>2002</v>
@@ -2070,81 +2070,81 @@
         <v>1994</v>
       </c>
       <c r="J32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K32" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L32" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="G33" s="2">
         <v>2000</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G34" s="2">
         <v>2011</v>
@@ -2156,13 +2156,13 @@
         <v>2003</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M34" s="2">
         <v>2.5</v>
@@ -2173,22 +2173,22 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G35" s="2">
         <v>2011</v>
@@ -2200,39 +2200,39 @@
         <v>2004</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="E36" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G36" s="2">
         <v>2011</v>
@@ -2244,13 +2244,13 @@
         <v>2003</v>
       </c>
       <c r="J36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K36" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L36" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M36" s="2">
         <v>3.9</v>
@@ -2261,66 +2261,66 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="G37" s="3">
         <v>1992</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G38" s="2">
         <v>1991</v>
@@ -2332,13 +2332,13 @@
         <v>1990</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M38" s="2">
         <v>49</v>
@@ -2349,22 +2349,22 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G39" s="2">
         <v>1991</v>
@@ -2376,19 +2376,19 @@
         <v>2011</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>